<commit_message>
FUNCTIONALITY: SchedulingUIFormat - Documented two existing test cases and wrote one new one. OverlayIdentifierDefault - Fixed a timing error.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step1/Scheduling/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step1/Scheduling/_Test_Suite_Statistics.xlsx
@@ -528,7 +528,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +620,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>7</v>
@@ -630,7 +630,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C$2:C36)</f>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -648,7 +648,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.94871794871794868</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Wrote two new test cases.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step1/Scheduling/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step1/Scheduling/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Title</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>SchedulingUIFormat</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Contains 1 partially automated test case.</t>
+  </si>
+  <si>
+    <t>Contains 4 partially automated test cases.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +161,74 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -528,7 +604,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,13 +677,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
@@ -617,20 +696,23 @@
         <v>13</v>
       </c>
       <c r="B4" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="3">
         <f>SUM($C$2:C36)</f>
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -639,7 +721,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B$2:B36)</f>
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -648,7 +730,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.92500000000000004</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -667,30 +749,30 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="D2:D50">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="9" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="9" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="6" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="14" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="13" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="12" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="11" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="10" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="9" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="8" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>